<commit_message>
Looking an alternative excel solution
</commit_message>
<xml_diff>
--- a/PQ_Challenge_196.xlsx
+++ b/PQ_Challenge_196.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B628EAC8-197C-4814-A13B-59AEB5450B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63598C9A-D442-4B6C-A5DB-6293BC860456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="13">
   <si>
     <t>Class</t>
   </si>
@@ -621,6 +645,450 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Right 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FEA0442-C601-4AC8-9451-CA9FF34A90FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1510030" y="593090"/>
+          <a:ext cx="749300" cy="542290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>RESULT</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Left 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1692F0D7-8007-47CE-B6E7-270F82642760}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1421130" y="114300"/>
+          <a:ext cx="844550" cy="497840"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1050" b="1"/>
+            <a:t>PROBLEM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>220762</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50495</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A person in a suit with his hands on his hips&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{403876B4-46B4-4174-A1DF-AFFC3A47320A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2971582" y="871220"/>
+          <a:ext cx="4035973" cy="8538210"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Thought Bubble: Cloud 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3199B2-74B3-4196-8121-408EAF88A925}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1160780" y="1943100"/>
+          <a:ext cx="3263900" cy="1809750"/>
+        </a:xfrm>
+        <a:prstGeom prst="cloudCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 53975"/>
+            <a:gd name="adj2" fmla="val -73389"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>Transpose the problem table into result table. Class will be populated under subjects and marks will be populated under headers Marks-Subject Name.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>732790</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="A close-up of several logos&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B04B9FE-B739-4106-8565-41DD0494E57A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4767580" y="2901950"/>
+          <a:ext cx="1002030" cy="615101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Right 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A9C6B2-814B-49A5-8366-ED7295A1FFA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1510030" y="593090"/>
+          <a:ext cx="749300" cy="542290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>RESULT</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Left 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D8E7AF-AA3B-4B3B-A326-093B764900A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1421130" y="114300"/>
+          <a:ext cx="844550" cy="497840"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1050" b="1"/>
+            <a:t>PROBLEM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -886,7 +1354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -1148,4 +1616,661 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025FEE32-F787-4259-BC21-6B69088EA6C9}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9">
+        <v>60</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14">
+        <v>8</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14">
+        <v>60</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9">
+        <v>90</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14">
+        <v>9</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
+        <v>70</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13">
+        <v>10</v>
+      </c>
+      <c r="G4" s="14">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14">
+        <v>10</v>
+      </c>
+      <c r="I4" s="14">
+        <v>10</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14">
+        <v>60</v>
+      </c>
+      <c r="L4" s="14">
+        <v>50</v>
+      </c>
+      <c r="M4" s="14">
+        <v>20</v>
+      </c>
+      <c r="N4" s="14">
+        <v>80</v>
+      </c>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>60</v>
+      </c>
+      <c r="F5" s="16">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17">
+        <v>11</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17">
+        <v>11</v>
+      </c>
+      <c r="K5" s="17">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17">
+        <v>100</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D8B0A4-7FD2-4AF8-B3E1-DA039A1BB7C9}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9">
+        <v>60</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14">
+        <v>8</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14">
+        <v>60</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9">
+        <v>90</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14">
+        <v>9</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
+        <v>70</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13">
+        <v>10</v>
+      </c>
+      <c r="G4" s="14">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14">
+        <v>10</v>
+      </c>
+      <c r="I4" s="14">
+        <v>10</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14">
+        <v>60</v>
+      </c>
+      <c r="L4" s="14">
+        <v>50</v>
+      </c>
+      <c r="M4" s="14">
+        <v>20</v>
+      </c>
+      <c r="N4" s="14">
+        <v>80</v>
+      </c>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>60</v>
+      </c>
+      <c r="F5" s="16">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17">
+        <v>11</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17">
+        <v>11</v>
+      </c>
+      <c r="K5" s="17">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17">
+        <v>100</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17:K20">_xlfn.LET(_xlpm.a,A2:A11,_xlpm.b,B2:B11,_xlpm.e,_xlfn.LAMBDA(_xlpm.x,_xlfn.XLOOKUP(_xlfn.UNIQUE(_xlpm.a)&amp;_xlfn.TOROW(_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.b))),_xlpm.a&amp;_xlpm.b,_xlpm.x,"")),_xlfn.HSTACK(_xlpm.e(_xlpm.a),_xlpm.e(C2:C11)))</f>
+        <v/>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18">
+        <v>70</v>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19">
+        <v>60</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19">
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <v>80</v>
+      </c>
+      <c r="K19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>